<commit_message>
Added Explore Cancel and DS close Scripts.
</commit_message>
<xml_diff>
--- a/Myles.xlsx
+++ b/Myles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14970" windowHeight="6525" tabRatio="733" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15555" windowHeight="6525" tabRatio="1000" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Myles" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,15 @@
     <sheet name="Swap-Car" sheetId="9" r:id="rId8"/>
     <sheet name="Invoice-Damage" sheetId="10" r:id="rId9"/>
     <sheet name="PromotionMaster" sheetId="11" r:id="rId10"/>
+    <sheet name="Explore-Cancel" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N20"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="127">
   <si>
     <t>City</t>
   </si>
@@ -140,12 +141,6 @@
     <t>admin.myles</t>
   </si>
   <si>
-    <t>6668815</t>
-  </si>
-  <si>
-    <t>8946858805</t>
-  </si>
-  <si>
     <t>12341234</t>
   </si>
   <si>
@@ -227,9 +222,6 @@
     <t>dropTime</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>LocWiseModelWise( Location Wise &amp; Model Wise)</t>
   </si>
   <si>
@@ -290,30 +282,15 @@
     <t>PaymentThrew</t>
   </si>
   <si>
-    <t>November 18, 2018</t>
-  </si>
-  <si>
-    <t>November 12, 2018</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
     <t>Location Wise</t>
   </si>
   <si>
-    <t>Rajouri garden- TDI Mall</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>24 Nov, 2018</t>
-  </si>
-  <si>
     <t>mannualChargingInfo</t>
   </si>
   <si>
@@ -359,49 +336,76 @@
     <t>18</t>
   </si>
   <si>
-    <t>Insta@1111</t>
-  </si>
-  <si>
     <t>Booking Modification</t>
   </si>
   <si>
-    <t>6669067</t>
-  </si>
-  <si>
-    <t>2212001111</t>
-  </si>
-  <si>
     <t>26</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>Etios - Standard</t>
-  </si>
-  <si>
     <t>Unlimited</t>
   </si>
   <si>
-    <t>6666698</t>
-  </si>
-  <si>
-    <t>6669062</t>
-  </si>
-  <si>
     <t>9610 DL1N</t>
   </si>
   <si>
     <t>8285335139</t>
   </si>
   <si>
-    <t>12345678</t>
-  </si>
-  <si>
-    <t>6669221</t>
-  </si>
-  <si>
-    <t>6669222</t>
+    <t>January 10, 2019</t>
+  </si>
+  <si>
+    <t>January 11, 2019</t>
+  </si>
+  <si>
+    <t>Mahipalpur</t>
+  </si>
+  <si>
+    <t>Aspire - Economy</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>19 Jan, 2019</t>
+  </si>
+  <si>
+    <t>8527463737</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Insta@3333</t>
+  </si>
+  <si>
+    <t>6672944</t>
+  </si>
+  <si>
+    <t>6672835</t>
+  </si>
+  <si>
+    <t>6672808</t>
+  </si>
+  <si>
+    <t>6672950</t>
+  </si>
+  <si>
+    <t>KmIn</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1152</t>
   </si>
 </sst>
 </file>
@@ -479,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -491,7 +495,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -798,7 +801,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +822,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>34</v>
@@ -849,39 +852,39 @@
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>123</v>
+      <c r="B2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
         <v>31</v>
@@ -890,10 +893,10 @@
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -907,8 +910,12 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1040,7 +1047,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,13 +1078,67 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1087,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,49 +1178,49 @@
         <v>34</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="G1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1170,59 +1231,60 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" t="s">
-        <v>92</v>
-      </c>
       <c r="O2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="Q2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1231,7 +1293,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1306,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E1" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,7 +1314,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>34</v>
@@ -1261,24 +1323,24 @@
         <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>123</v>
+      <c r="B3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1292,7 +1354,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,18 +1391,18 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1350,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1433,7 @@
         <v>32</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>34</v>
@@ -1380,42 +1442,42 @@
         <v>35</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>123</v>
+      <c r="B2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1428,7 +1490,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,22 +1520,22 @@
         <v>35</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1484,30 +1546,30 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1515,15 +1577,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -1536,8 +1602,11 @@
       <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1545,15 +1614,18 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1564,7 +1636,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,12 +1648,12 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>34</v>
@@ -1590,41 +1662,41 @@
         <v>35</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
         <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3" display="Insta@2021"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1635,7 +1707,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,25 +1738,25 @@
         <v>35</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1695,36 +1767,36 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added browser optimization code.
</commit_message>
<xml_diff>
--- a/Myles.xlsx
+++ b/Myles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15555" windowHeight="6525" tabRatio="1000" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15555" windowHeight="6525" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="Myles" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Explore-Cancel" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O20"/>
+  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="131">
   <si>
     <t>City</t>
   </si>
@@ -120,9 +120,6 @@
     <t>23:00</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>S.No.</t>
   </si>
   <si>
@@ -381,31 +378,46 @@
     <t>January</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
     <t>Insta@3333</t>
   </si>
   <si>
-    <t>6672944</t>
-  </si>
-  <si>
-    <t>6672835</t>
-  </si>
-  <si>
-    <t>6672808</t>
-  </si>
-  <si>
-    <t>6672950</t>
-  </si>
-  <si>
     <t>KmIn</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>1152</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>6672965</t>
+  </si>
+  <si>
+    <t>6673038</t>
+  </si>
+  <si>
+    <t>6673039</t>
+  </si>
+  <si>
+    <t>6673040</t>
+  </si>
+  <si>
+    <t>6673041</t>
+  </si>
+  <si>
+    <t>6673042</t>
+  </si>
+  <si>
+    <t>6673043</t>
+  </si>
+  <si>
+    <t>6673044</t>
+  </si>
+  <si>
+    <t>6673045</t>
+  </si>
+  <si>
+    <t>6673046</t>
   </si>
 </sst>
 </file>
@@ -800,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +834,10 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -852,10 +864,10 @@
         <v>7</v>
       </c>
       <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -863,40 +875,40 @@
         <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -911,10 +923,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1060,13 +1072,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D1" s="5"/>
     </row>
@@ -1075,16 +1087,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1106,16 +1118,16 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1126,19 +1138,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
         <v>121</v>
       </c>
       <c r="F2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1169,58 +1181,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="R1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1228,60 +1240,60 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="N2" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>111</v>
       </c>
-      <c r="O2" t="s">
-        <v>112</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1293,7 +1305,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,24 +1318,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E1" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1331,16 +1343,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1368,19 +1380,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1388,21 +1400,21 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1413,7 +1425,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,28 +1442,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1459,25 +1471,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1502,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,34 +1520,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="I1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1543,33 +1555,33 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1579,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1591,19 +1603,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1611,21 +1623,21 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
         <v>119</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1650,25 +1662,25 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1676,27 +1688,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1726,37 +1738,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="G1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1764,39 +1776,39 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new booking code.
</commit_message>
<xml_diff>
--- a/Myles.xlsx
+++ b/Myles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15555" windowHeight="6525" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15555" windowHeight="6525" tabRatio="1000" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Myles" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Explore-Cancel" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K20"/>
+  <oleSize ref="A1:I20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="122">
   <si>
     <t>City</t>
   </si>
@@ -390,42 +390,14 @@
     <t>12345678</t>
   </si>
   <si>
-    <t>6672965</t>
-  </si>
-  <si>
-    <t>6673038</t>
-  </si>
-  <si>
-    <t>6673039</t>
-  </si>
-  <si>
-    <t>6673040</t>
-  </si>
-  <si>
-    <t>6673041</t>
-  </si>
-  <si>
-    <t>6673042</t>
-  </si>
-  <si>
-    <t>6673043</t>
-  </si>
-  <si>
-    <t>6673044</t>
-  </si>
-  <si>
-    <t>6673045</t>
-  </si>
-  <si>
-    <t>6673046</t>
+    <t>6673103</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,21 +784,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1064,10 +1036,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1096,7 +1068,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1112,8 +1084,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1122,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1166,17 +1138,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="49.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1293,7 +1265,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId66"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1310,10 +1282,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1321,7 @@
         <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
         <v>102</v>
@@ -1371,11 +1343,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,15 +1378,15 @@
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1430,14 +1402,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1477,7 +1449,7 @@
         <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>116</v>
@@ -1501,21 +1473,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1561,7 +1533,7 @@
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
         <v>46</v>
@@ -1581,7 +1553,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1597,8 +1569,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1629,7 +1601,7 @@
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
         <v>119</v>
@@ -1637,7 +1609,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1653,11 +1625,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1666,7 @@
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
         <v>80</v>
@@ -1708,7 +1680,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1724,16 +1696,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1782,7 +1754,7 @@
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>99</v>
@@ -1808,7 +1780,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId65"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>